<commit_message>
feat: Add badge generation functionality
- Implements a new `badges.py` script to create event badges for various roles.
- Integrates badge generation into the main application flow.
- Renames `generateCertificates` to `generate` in `awards.py` and `participants.py` for consistency.
- Adds badge assets and VS Code settings.
</commit_message>
<xml_diff>
--- a/dummy_list.xlsx
+++ b/dummy_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshianaseri/Arshia/FIRA 2025/Certificates/@github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshianaseri/Arshia/Projects/FIRA_Certificate_Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA83EA86-8768-C74B-BF85-0E8B0E006D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64FDFD0-E0E1-8D4D-BFAC-907F09872B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="409">
   <si>
     <t>Name</t>
   </si>
@@ -1262,9 +1262,6 @@
   </si>
   <si>
     <t>Best Performance Certificate</t>
-  </si>
-  <si>
-    <t>Division</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1308,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1620,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4469,8 +4466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D033618C-D15E-9D45-BFC9-137EEFE8290A}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4489,7 +4486,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>409</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>

</xml_diff>